<commit_message>
added test agreement, fixed user update
</commit_message>
<xml_diff>
--- a/data/data2.xlsx
+++ b/data/data2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Data/move_on/django/projects/myproject/myproject/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{514C8102-94EE-434E-B55A-CA7D562E0D32}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06F6437D-9411-F64D-B856-F2553DA96F64}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="820" windowWidth="27640" windowHeight="15840" xr2:uid="{42A4FE2A-8365-3842-ACC8-D74453F99B5D}"/>
   </bookViews>
@@ -521,7 +521,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>